<commit_message>
Fixes in tests and layout
</commit_message>
<xml_diff>
--- a/tests/test_examples/pollution_data_test_3.xlsx
+++ b/tests/test_examples/pollution_data_test_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51ae962a39f43cd0/Pulpit/Marcysia/github/visualisation_geographic_data/tests/test_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{32D97925-EDF2-4026-9521-DCAA707596EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB96BDF-9C44-455F-A398-F8748EDD4416}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{32D97925-EDF2-4026-9521-DCAA707596EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D74BDF7-9136-4333-91AE-016AF04E83B6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{464988A6-2CE5-4FD1-850F-A329DDD75F44}"/>
+    <workbookView xWindow="3672" yWindow="2280" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{464988A6-2CE5-4FD1-850F-A329DDD75F44}"/>
   </bookViews>
   <sheets>
     <sheet name="data2020" sheetId="1" r:id="rId1"/>
@@ -918,6 +918,14 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
@@ -2598,7 +2606,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2632,7 +2640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="24">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -2753,7 +2761,7 @@
         <v>4.75</v>
       </c>
       <c r="F6" s="3">
-        <v>68.91</v>
+        <v>0</v>
       </c>
       <c r="G6" s="3">
         <v>73.14</v>
@@ -2762,7 +2770,7 @@
         <v>157.88</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="24">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2788,7 +2796,7 @@
         <v>430.74</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="24">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -2840,7 +2848,7 @@
         <v>82.56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="24">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2860,7 +2868,7 @@
         <v>17.78</v>
       </c>
       <c r="G10" s="3">
-        <v>29.19</v>
+        <v>0</v>
       </c>
       <c r="H10" s="3">
         <v>131.86000000000001</v>
@@ -2903,7 +2911,7 @@
         <v>13571.28</v>
       </c>
       <c r="D12" s="3">
-        <v>66.48</v>
+        <v>0</v>
       </c>
       <c r="E12" s="3">
         <v>3.33</v>
@@ -2944,7 +2952,7 @@
         <v>241.36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="24">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -2996,7 +3004,7 @@
         <v>97.85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="24">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>